<commit_message>
feat: Add PyCaret-based 2026 headcount prediction to Dashboard
- Added _predict_headcount_2026() method using linear regression
- Integrated headcount prediction into predict_wage_increase() response
- Updated frontend Dashboard to display 2026 predicted headcount
- Replaced economic indicators card with headcount prediction display
- Shows predicted headcount, growth rate, and model details
- Headcount prediction based on historical trend analysis

🤖 Generated with [Claude Code](https://claude.ai/code)

Co-Authored-By: Claude <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/Hwaseung feature.xlsx
+++ b/Hwaseung feature.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hanskim/Projects/Hwaseung/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7D35F69-D9BB-D34E-9337-31C3A33D63B6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A360E7E-87C8-A948-96CB-69C9AD10D078}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2940" yWindow="2520" windowWidth="27400" windowHeight="15920" xr2:uid="{B683F346-9D45-4A95-AA5F-47F0780B8E2B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>eng</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -106,14 +106,6 @@
   </si>
   <si>
     <t>exchange_rate_change_krw</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>-</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>2025 (예측치)</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -280,7 +272,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -301,15 +293,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="38" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="3" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -663,13 +646,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{903D7150-8BC5-4AA6-BD64-90512E4F0D66}">
-  <dimension ref="A1:P14"/>
+  <dimension ref="A1:P8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="M7" sqref="M7"/>
+      <selection pane="bottomRight" activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -712,22 +695,22 @@
         <v>16</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="M1" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="4" t="s">
-        <v>32</v>
-      </c>
       <c r="P1" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:16">
@@ -762,574 +745,274 @@
         <v>6</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O2" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:16">
       <c r="A3" s="5">
-        <v>2015</v>
+        <v>2021</v>
       </c>
       <c r="B3" s="6">
-        <v>0.17</v>
+        <v>1.04</v>
       </c>
       <c r="C3" s="6">
-        <v>1.7000000000000001E-2</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="D3" s="6">
-        <v>-9.8000000000000004E-2</v>
+        <v>0.24199999999999999</v>
       </c>
       <c r="E3" s="6">
-        <v>-4.1000000000000002E-2</v>
+        <v>0.222</v>
       </c>
       <c r="F3" s="6">
-        <v>2.9000000000000001E-2</v>
+        <v>4.5999999999999999E-2</v>
       </c>
       <c r="G3" s="6">
-        <v>7.0000000000000001E-3</v>
+        <v>2.5000000000000001E-2</v>
       </c>
       <c r="H3" s="6">
-        <v>7.4800000000000005E-2</v>
+        <v>-2.9499999999999998E-2</v>
       </c>
       <c r="I3" s="6">
-        <v>719.86290322580646</v>
+        <v>2943.38</v>
       </c>
       <c r="J3" s="6">
-        <v>-85.671999999999997</v>
-      </c>
-      <c r="K3" s="10">
+        <v>39.097999999999999</v>
+      </c>
+      <c r="K3" s="7">
         <v>1</v>
       </c>
-      <c r="L3" s="10">
+      <c r="L3" s="7">
         <v>1</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="7">
         <v>1</v>
       </c>
-      <c r="N3" s="10">
+      <c r="N3" s="7">
         <v>1</v>
       </c>
-      <c r="O3" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="P3" s="7" t="s">
-        <v>20</v>
+      <c r="O3" s="7">
+        <v>1</v>
+      </c>
+      <c r="P3" s="8">
+        <v>754</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="5">
-        <v>2016</v>
+        <v>2022</v>
       </c>
       <c r="B4" s="6">
-        <v>0.25</v>
+        <v>0.59</v>
       </c>
       <c r="C4" s="6">
         <v>0.05</v>
       </c>
       <c r="D4" s="6">
-        <v>-0.113</v>
+        <v>0.41799999999999998</v>
       </c>
       <c r="E4" s="6">
-        <v>-4.3999999999999997E-2</v>
+        <v>1.4E-2</v>
       </c>
       <c r="F4" s="6">
-        <v>3.2000000000000001E-2</v>
+        <v>2.7E-2</v>
       </c>
       <c r="G4" s="6">
-        <v>0.01</v>
+        <v>5.0999999999999997E-2</v>
       </c>
       <c r="H4" s="6">
-        <v>2.5600000000000001E-2</v>
+        <v>0.1298</v>
       </c>
       <c r="I4" s="6">
-        <v>673.12</v>
+        <v>1933.8178137651821</v>
       </c>
       <c r="J4" s="6">
-        <v>-18.768000000000001</v>
-      </c>
-      <c r="K4" s="10">
-        <v>1</v>
-      </c>
-      <c r="L4" s="10">
-        <v>1</v>
-      </c>
-      <c r="M4" s="10">
-        <v>1</v>
-      </c>
-      <c r="N4" s="10">
-        <v>1</v>
-      </c>
-      <c r="O4" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P4" s="8" t="s">
-        <v>20</v>
+        <v>28.361999999999998</v>
+      </c>
+      <c r="K4" s="7">
+        <v>1.3008749691978805</v>
+      </c>
+      <c r="L4" s="7">
+        <v>1.9070783084721636</v>
+      </c>
+      <c r="M4" s="7">
+        <v>1.0807089494261799</v>
+      </c>
+      <c r="N4" s="7">
+        <v>1.3213773946782479</v>
+      </c>
+      <c r="O4" s="7">
+        <v>1.1328266503779481</v>
+      </c>
+      <c r="P4" s="8">
+        <v>591</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="5">
-        <v>2017</v>
+        <v>2023</v>
       </c>
       <c r="B5" s="6">
-        <v>0.11</v>
+        <v>0.33</v>
       </c>
       <c r="C5" s="6">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="D5" s="6">
+        <v>0.127</v>
+      </c>
+      <c r="E5" s="6">
+        <v>-0.182</v>
+      </c>
+      <c r="F5" s="6">
+        <v>1.6E-2</v>
+      </c>
+      <c r="G5" s="6">
+        <v>3.5999999999999997E-2</v>
+      </c>
+      <c r="H5" s="6">
         <v>1.0999999999999999E-2</v>
       </c>
-      <c r="D5" s="6">
-        <v>0.217</v>
-      </c>
-      <c r="E5" s="6">
-        <v>-5.1999999999999998E-3</v>
-      </c>
-      <c r="F5" s="6">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="G5" s="6">
-        <v>1.9E-2</v>
-      </c>
-      <c r="H5" s="6">
-        <v>-2.63E-2</v>
-      </c>
       <c r="I5" s="6">
-        <v>1145.2289156626507</v>
+        <v>1378.3709677419354</v>
       </c>
       <c r="J5" s="6">
-        <v>17.556000000000001</v>
-      </c>
-      <c r="K5" s="10">
-        <v>1</v>
-      </c>
-      <c r="L5" s="10">
-        <v>1</v>
-      </c>
-      <c r="M5" s="10">
-        <v>1</v>
-      </c>
-      <c r="N5" s="10">
-        <v>1</v>
-      </c>
-      <c r="O5" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="P5" s="8" t="s">
-        <v>20</v>
+        <v>-20.530999999999999</v>
+      </c>
+      <c r="K5" s="7">
+        <v>1.0345389737155919</v>
+      </c>
+      <c r="L5" s="7">
+        <v>2.049871532681554</v>
+      </c>
+      <c r="M5" s="7">
+        <v>1.0403181491874618</v>
+      </c>
+      <c r="N5" s="7">
+        <v>1.0544653731293481</v>
+      </c>
+      <c r="O5" s="7">
+        <v>1.3456087306832234</v>
+      </c>
+      <c r="P5" s="8">
+        <v>606</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="5">
-        <v>2018</v>
+        <v>2024</v>
       </c>
       <c r="B6" s="6">
-        <v>0.65</v>
+        <v>0.21</v>
       </c>
       <c r="C6" s="6">
-        <v>-1.0999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="D6" s="6">
-        <v>-1.9E-2</v>
+        <v>-1E-3</v>
       </c>
       <c r="E6" s="6">
-        <v>-0.161</v>
+        <v>3.4000000000000002E-2</v>
       </c>
       <c r="F6" s="6">
-        <v>3.2000000000000001E-2</v>
+        <v>0.02</v>
       </c>
       <c r="G6" s="6">
-        <v>1.4999999999999999E-2</v>
+        <v>2.3E-2</v>
       </c>
       <c r="H6" s="6">
-        <v>-2.6100000000000002E-2</v>
+        <v>4.4900000000000002E-2</v>
       </c>
       <c r="I6" s="6">
-        <v>1352.6279999999999</v>
+        <v>1754.0357142857142</v>
       </c>
       <c r="J6" s="6">
-        <v>23.643000000000001</v>
-      </c>
-      <c r="K6" s="10">
-        <v>1</v>
-      </c>
-      <c r="L6" s="10">
-        <v>1</v>
-      </c>
-      <c r="M6" s="10">
-        <v>1</v>
-      </c>
-      <c r="N6" s="10">
-        <v>1</v>
-      </c>
-      <c r="O6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="P6" s="9" t="s">
-        <v>20</v>
+        <v>-2.8929999999999998</v>
+      </c>
+      <c r="K6" s="7">
+        <v>1.0389022583676739</v>
+      </c>
+      <c r="L6" s="7">
+        <v>0.98631097479879426</v>
+      </c>
+      <c r="M6" s="7">
+        <v>1.0999086053900509</v>
+      </c>
+      <c r="N6" s="7">
+        <v>0.98251048990880263</v>
+      </c>
+      <c r="O6" s="7">
+        <v>1.150527862138456</v>
+      </c>
+      <c r="P6" s="8">
+        <v>600</v>
       </c>
     </row>
     <row r="7" spans="1:16">
-      <c r="A7" s="5">
-        <v>2019</v>
+      <c r="A7" s="9">
+        <v>2025</v>
       </c>
       <c r="B7" s="6">
-        <v>0.09</v>
-      </c>
-      <c r="C7" s="6">
-        <v>-2.1000000000000001E-2</v>
-      </c>
-      <c r="D7" s="6">
-        <v>-7.0999999999999994E-2</v>
-      </c>
-      <c r="E7" s="6">
-        <v>-9.2999999999999999E-2</v>
+        <v>0.18</v>
+      </c>
+      <c r="C7" s="10">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D7" s="11">
+        <v>0.1997999999999962</v>
+      </c>
+      <c r="E7" s="11">
+        <v>-1.3866666666668692E-3</v>
       </c>
       <c r="F7" s="6">
-        <v>2.3E-2</v>
+        <v>0.01</v>
       </c>
       <c r="G7" s="6">
-        <v>4.0000000000000001E-3</v>
+        <v>1.7999999999999999E-2</v>
       </c>
       <c r="H7" s="6">
-        <v>5.9400000000000001E-2</v>
+        <v>4.2000000000000003E-2</v>
       </c>
       <c r="I7" s="6">
-        <v>1352.8119999999999</v>
+        <v>1451.452380952381</v>
       </c>
       <c r="J7" s="6">
-        <v>-13.04</v>
-      </c>
-      <c r="K7" s="10">
-        <v>1</v>
-      </c>
-      <c r="L7" s="10">
-        <v>1</v>
-      </c>
-      <c r="M7" s="10">
-        <v>1</v>
-      </c>
-      <c r="N7" s="10">
-        <v>1</v>
-      </c>
-      <c r="O7" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="P7" s="9" t="s">
-        <v>20</v>
-      </c>
+        <v>-13.712</v>
+      </c>
+      <c r="K7" s="7">
+        <v>1.1236645562316938</v>
+      </c>
+      <c r="L7" s="7">
+        <v>1.3772631009287266</v>
+      </c>
+      <c r="M7" s="7">
+        <v>1.0502508820127165</v>
+      </c>
+      <c r="N7" s="7">
+        <v>1.1436643896280407</v>
+      </c>
+      <c r="O7" s="7">
+        <v>1.1494874677704476</v>
+      </c>
+      <c r="P7" s="12"/>
     </row>
     <row r="8" spans="1:16">
-      <c r="A8" s="5">
-        <v>2020</v>
-      </c>
-      <c r="B8" s="6">
-        <v>0.47</v>
-      </c>
-      <c r="C8" s="6">
-        <v>-0.152</v>
-      </c>
-      <c r="D8" s="6">
-        <v>-0.13100000000000001</v>
-      </c>
-      <c r="E8" s="6">
-        <v>-0.08</v>
-      </c>
-      <c r="F8" s="6">
-        <v>-7.0000000000000001E-3</v>
-      </c>
-      <c r="G8" s="6">
-        <v>5.0000000000000001E-3</v>
-      </c>
-      <c r="H8" s="6">
-        <v>1.15E-2</v>
-      </c>
-      <c r="I8" s="6">
-        <v>1060.9554655870445</v>
-      </c>
-      <c r="J8" s="6">
-        <v>-46.771999999999998</v>
-      </c>
-      <c r="K8" s="10">
-        <v>1</v>
-      </c>
-      <c r="L8" s="10">
-        <v>1</v>
-      </c>
-      <c r="M8" s="10">
-        <v>1</v>
-      </c>
-      <c r="N8" s="10">
-        <v>1</v>
-      </c>
-      <c r="O8" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="P8" s="9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16">
-      <c r="A9" s="5">
-        <v>2021</v>
-      </c>
-      <c r="B9" s="6">
-        <v>1.04</v>
-      </c>
-      <c r="C9" s="6">
-        <v>2.5999999999999999E-2</v>
-      </c>
-      <c r="D9" s="6">
-        <v>0.24199999999999999</v>
-      </c>
-      <c r="E9" s="6">
-        <v>0.222</v>
-      </c>
-      <c r="F9" s="6">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="G9" s="6">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="H9" s="6">
-        <v>-2.9499999999999998E-2</v>
-      </c>
-      <c r="I9" s="6">
-        <v>2943.38</v>
-      </c>
-      <c r="J9" s="6">
-        <v>39.097999999999999</v>
-      </c>
-      <c r="K9" s="10">
-        <v>1</v>
-      </c>
-      <c r="L9" s="10">
-        <v>1</v>
-      </c>
-      <c r="M9" s="10">
-        <v>1</v>
-      </c>
-      <c r="N9" s="10">
-        <v>1</v>
-      </c>
-      <c r="O9" s="10">
-        <v>1</v>
-      </c>
-      <c r="P9" s="11">
-        <v>754</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16">
-      <c r="A10" s="5">
-        <v>2022</v>
-      </c>
-      <c r="B10" s="6">
-        <v>0.59</v>
-      </c>
-      <c r="C10" s="6">
-        <v>0.05</v>
-      </c>
-      <c r="D10" s="6">
-        <v>0.41799999999999998</v>
-      </c>
-      <c r="E10" s="6">
-        <v>1.4E-2</v>
-      </c>
-      <c r="F10" s="6">
-        <v>2.7E-2</v>
-      </c>
-      <c r="G10" s="6">
-        <v>5.0999999999999997E-2</v>
-      </c>
-      <c r="H10" s="6">
-        <v>0.1298</v>
-      </c>
-      <c r="I10" s="6">
-        <v>1933.8178137651821</v>
-      </c>
-      <c r="J10" s="6">
-        <v>28.361999999999998</v>
-      </c>
-      <c r="K10" s="10">
-        <v>1.3008749691978805</v>
-      </c>
-      <c r="L10" s="10">
-        <v>1.9070783084721636</v>
-      </c>
-      <c r="M10" s="10">
-        <v>1.0807089494261799</v>
-      </c>
-      <c r="N10" s="10">
-        <v>1.3213773946782479</v>
-      </c>
-      <c r="O10" s="10">
-        <v>1.1328266503779481</v>
-      </c>
-      <c r="P10" s="11">
-        <v>591</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16">
-      <c r="A11" s="5">
-        <v>2023</v>
-      </c>
-      <c r="B11" s="6">
-        <v>0.33</v>
-      </c>
-      <c r="C11" s="6">
-        <v>4.8000000000000001E-2</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0.127</v>
-      </c>
-      <c r="E11" s="6">
-        <v>-0.182</v>
-      </c>
-      <c r="F11" s="6">
-        <v>1.6E-2</v>
-      </c>
-      <c r="G11" s="6">
-        <v>3.5999999999999997E-2</v>
-      </c>
-      <c r="H11" s="6">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="I11" s="6">
-        <v>1378.3709677419354</v>
-      </c>
-      <c r="J11" s="6">
-        <v>-20.530999999999999</v>
-      </c>
-      <c r="K11" s="10">
-        <v>1.0345389737155919</v>
-      </c>
-      <c r="L11" s="10">
-        <v>2.049871532681554</v>
-      </c>
-      <c r="M11" s="10">
-        <v>1.0403181491874618</v>
-      </c>
-      <c r="N11" s="10">
-        <v>1.0544653731293481</v>
-      </c>
-      <c r="O11" s="10">
-        <v>1.3456087306832234</v>
-      </c>
-      <c r="P11" s="11">
-        <v>606</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16">
-      <c r="A12" s="5">
-        <v>2024</v>
-      </c>
-      <c r="B12" s="6">
-        <v>0.21</v>
-      </c>
-      <c r="C12" s="6">
-        <v>2.3E-2</v>
-      </c>
-      <c r="D12" s="6">
-        <v>-1E-3</v>
-      </c>
-      <c r="E12" s="6">
-        <v>3.4000000000000002E-2</v>
-      </c>
-      <c r="F12" s="6">
-        <v>0.02</v>
-      </c>
-      <c r="G12" s="6">
-        <v>2.3E-2</v>
-      </c>
-      <c r="H12" s="6">
-        <v>4.4900000000000002E-2</v>
-      </c>
-      <c r="I12" s="6">
-        <v>1754.0357142857142</v>
-      </c>
-      <c r="J12" s="6">
-        <v>-2.8929999999999998</v>
-      </c>
-      <c r="K12" s="10">
-        <v>1.0389022583676739</v>
-      </c>
-      <c r="L12" s="10">
-        <v>0.98631097479879426</v>
-      </c>
-      <c r="M12" s="10">
-        <v>1.0999086053900509</v>
-      </c>
-      <c r="N12" s="10">
-        <v>0.98251048990880263</v>
-      </c>
-      <c r="O12" s="10">
-        <v>1.150527862138456</v>
-      </c>
-      <c r="P12" s="11">
-        <v>600</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16">
-      <c r="A13" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="6">
-        <v>0.18</v>
-      </c>
-      <c r="C13" s="13">
-        <v>3.3000000000000002E-2</v>
-      </c>
-      <c r="D13" s="14">
-        <v>0.1997999999999962</v>
-      </c>
-      <c r="E13" s="14">
-        <v>-1.3866666666668692E-3</v>
-      </c>
-      <c r="F13" s="6">
-        <v>0.01</v>
-      </c>
-      <c r="G13" s="6">
-        <v>1.7999999999999999E-2</v>
-      </c>
-      <c r="H13" s="6">
-        <v>4.2000000000000003E-2</v>
-      </c>
-      <c r="I13" s="6">
-        <v>1451.452380952381</v>
-      </c>
-      <c r="J13" s="6">
-        <v>-13.712</v>
-      </c>
-      <c r="K13" s="10">
-        <v>1.1236645562316938</v>
-      </c>
-      <c r="L13" s="10">
-        <v>1.3772631009287266</v>
-      </c>
-      <c r="M13" s="10">
-        <v>1.0502508820127165</v>
-      </c>
-      <c r="N13" s="10">
-        <v>1.1436643896280407</v>
-      </c>
-      <c r="O13" s="10">
-        <v>1.1494874677704476</v>
-      </c>
-      <c r="P13" s="15"/>
-    </row>
-    <row r="14" spans="1:16">
-      <c r="P14" s="1"/>
+      <c r="P8" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>